<commit_message>
Added the data provider for the tests. Updating the test results in one excel sheet, for comparison
</commit_message>
<xml_diff>
--- a/src/test/resources/com/testvagrant/excel/testData.xlsx
+++ b/src/test/resources/com/testvagrant/excel/testData.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mayuresh\Learning\Programming\Java\Workspace\WeatherComparator\src\test\resources\com\testvagrant\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3FB3F4-631C-4C88-91BC-F0B8C77BFD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7A3E58-7ACF-47AC-A28A-1AC724697007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Locations" sheetId="3" r:id="rId1"/>
-    <sheet name="SiteWeatherTest" sheetId="4" r:id="rId2"/>
-    <sheet name="APIWeatherTest" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,60 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
-  <si>
-    <t>RunMode</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Automation Testing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Pune</t>
   </si>
   <si>
-    <t>mayuresh.ahirrao@gmail.com</t>
-  </si>
-  <si>
-    <t>Mayur31885</t>
-  </si>
-  <si>
-    <t>SearchKey</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Place</t>
   </si>
   <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
     <t>State</t>
   </si>
   <si>
-    <t>ConuntryCode</t>
-  </si>
-  <si>
     <t>Maharashtra</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>New York</t>
   </si>
 </sst>
 </file>
@@ -431,136 +405,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB85A169-7D39-445D-A135-2D5126E7430C}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>